<commit_message>
Construct Execution tree (physical plan)
Construct tree of series of computing group by by resorting in some
nodes
</commit_message>
<xml_diff>
--- a/docs/second_step_simplex_table.xlsx
+++ b/docs/second_step_simplex_table.xlsx
@@ -124,7 +124,7 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="4" x14ac:knownFonts="1">
+  <fonts count="5" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -152,6 +152,14 @@
     </font>
     <font>
       <sz val="11"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <charset val="204"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="4"/>
       <name val="Calibri"/>
       <family val="2"/>
       <charset val="204"/>
@@ -207,17 +215,14 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="11">
+  <cellXfs count="13">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -231,6 +236,21 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
   </cellXfs>
@@ -537,164 +557,167 @@
   <dimension ref="A1:AA13"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="U11" sqref="U11"/>
+      <selection activeCell="T12" sqref="T12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="7" max="7" width="9.140625" customWidth="1"/>
+  </cols>
   <sheetData>
     <row r="1" spans="1:27" x14ac:dyDescent="0.25">
-      <c r="C1" s="2">
+      <c r="C1" s="1">
         <v>0</v>
       </c>
-      <c r="D1" s="2">
-        <v>1</v>
-      </c>
-      <c r="E1" s="2">
+      <c r="D1" s="1">
+        <v>1</v>
+      </c>
+      <c r="E1" s="1">
         <v>2</v>
       </c>
-      <c r="F1" s="2">
+      <c r="F1" s="1">
         <v>3</v>
       </c>
-      <c r="G1" s="2">
+      <c r="G1" s="1">
         <v>4</v>
       </c>
-      <c r="H1" s="2">
+      <c r="H1" s="1">
         <v>5</v>
       </c>
-      <c r="I1" s="2">
+      <c r="I1" s="1">
         <v>6</v>
       </c>
-      <c r="J1" s="2">
+      <c r="J1" s="1">
         <v>7</v>
       </c>
-      <c r="K1" s="2">
+      <c r="K1" s="1">
         <v>8</v>
       </c>
-      <c r="L1" s="2">
+      <c r="L1" s="1">
         <v>9</v>
       </c>
-      <c r="M1" s="2">
+      <c r="M1" s="1">
         <v>10</v>
       </c>
-      <c r="N1" s="2">
+      <c r="N1" s="1">
         <v>11</v>
       </c>
-      <c r="O1" s="2">
+      <c r="O1" s="1">
         <v>12</v>
       </c>
-      <c r="P1" s="2">
+      <c r="P1" s="1">
         <v>13</v>
       </c>
-      <c r="Q1" s="2">
+      <c r="Q1" s="1">
         <v>14</v>
       </c>
-      <c r="R1" s="2">
+      <c r="R1" s="1">
         <v>15</v>
       </c>
-      <c r="S1" s="2">
+      <c r="S1" s="1">
         <v>16</v>
       </c>
-      <c r="T1" s="2">
+      <c r="T1" s="1">
         <v>17</v>
       </c>
-      <c r="U1" s="2">
+      <c r="U1" s="1">
         <v>18</v>
       </c>
-      <c r="V1" s="2">
+      <c r="V1" s="1">
         <v>19</v>
       </c>
-      <c r="W1" s="2">
+      <c r="W1" s="1">
         <v>20</v>
       </c>
-      <c r="X1" s="2">
+      <c r="X1" s="1">
         <v>21</v>
       </c>
-      <c r="Y1" s="2">
+      <c r="Y1" s="1">
         <v>22</v>
       </c>
-      <c r="Z1" s="2">
+      <c r="Z1" s="1">
         <v>23</v>
       </c>
-      <c r="AA1" s="2">
+      <c r="AA1" s="1">
         <v>24</v>
       </c>
     </row>
     <row r="2" spans="1:27" x14ac:dyDescent="0.25">
-      <c r="D2" t="s">
+      <c r="D2" s="8" t="s">
         <v>4</v>
       </c>
-      <c r="E2" t="s">
+      <c r="E2" s="8" t="s">
         <v>5</v>
       </c>
-      <c r="F2" t="s">
+      <c r="F2" s="8" t="s">
         <v>6</v>
       </c>
-      <c r="G2" t="s">
+      <c r="G2" s="8" t="s">
         <v>7</v>
       </c>
-      <c r="H2" t="s">
+      <c r="H2" s="8" t="s">
         <v>8</v>
       </c>
-      <c r="I2" s="3" t="s">
+      <c r="I2" s="9" t="s">
         <v>9</v>
       </c>
-      <c r="J2" t="s">
+      <c r="J2" s="8" t="s">
         <v>4</v>
       </c>
-      <c r="K2" t="s">
+      <c r="K2" s="8" t="s">
         <v>5</v>
       </c>
-      <c r="L2" t="s">
+      <c r="L2" s="8" t="s">
         <v>6</v>
       </c>
-      <c r="M2" t="s">
+      <c r="M2" s="8" t="s">
         <v>7</v>
       </c>
-      <c r="N2" t="s">
+      <c r="N2" s="8" t="s">
         <v>8</v>
       </c>
-      <c r="O2" s="3" t="s">
+      <c r="O2" s="9" t="s">
         <v>9</v>
       </c>
-      <c r="P2" s="1" t="s">
+      <c r="P2" s="8" t="s">
         <v>4</v>
       </c>
-      <c r="Q2" s="1" t="s">
+      <c r="Q2" s="8" t="s">
         <v>5</v>
       </c>
-      <c r="R2" s="1" t="s">
+      <c r="R2" s="8" t="s">
         <v>6</v>
       </c>
-      <c r="S2" s="1" t="s">
+      <c r="S2" s="8" t="s">
         <v>7</v>
       </c>
-      <c r="T2" s="1" t="s">
+      <c r="T2" s="8" t="s">
         <v>8</v>
       </c>
-      <c r="U2" s="5" t="s">
+      <c r="U2" s="9" t="s">
         <v>9</v>
       </c>
-      <c r="V2" t="s">
+      <c r="V2" s="8" t="s">
         <v>4</v>
       </c>
-      <c r="W2" t="s">
+      <c r="W2" s="8" t="s">
         <v>5</v>
       </c>
-      <c r="X2" t="s">
+      <c r="X2" s="8" t="s">
         <v>6</v>
       </c>
-      <c r="Y2" t="s">
+      <c r="Y2" s="8" t="s">
         <v>7</v>
       </c>
-      <c r="Z2" t="s">
+      <c r="Z2" s="8" t="s">
         <v>8</v>
       </c>
-      <c r="AA2" s="3" t="s">
+      <c r="AA2" s="9" t="s">
         <v>9</v>
       </c>
     </row>
     <row r="3" spans="1:27" x14ac:dyDescent="0.25">
-      <c r="A3" s="2">
+      <c r="A3" s="1">
         <v>0</v>
       </c>
       <c r="B3" t="s">
@@ -703,41 +726,41 @@
       <c r="C3">
         <v>1</v>
       </c>
-      <c r="D3" s="2">
-        <v>1</v>
-      </c>
-      <c r="E3" s="2"/>
-      <c r="F3" s="2">
-        <v>1</v>
-      </c>
-      <c r="G3" s="2">
-        <v>1</v>
-      </c>
-      <c r="H3" s="2"/>
-      <c r="I3" s="4">
-        <v>1</v>
-      </c>
-      <c r="J3" s="2"/>
-      <c r="K3" s="2"/>
-      <c r="L3" s="2"/>
-      <c r="M3" s="2"/>
-      <c r="N3" s="2"/>
-      <c r="O3" s="4"/>
-      <c r="P3" s="2"/>
-      <c r="Q3" s="2"/>
-      <c r="R3" s="2"/>
-      <c r="S3" s="2"/>
-      <c r="T3" s="2"/>
-      <c r="U3" s="4"/>
-      <c r="V3" s="2"/>
-      <c r="W3" s="2"/>
-      <c r="X3" s="2"/>
-      <c r="Y3" s="2"/>
-      <c r="Z3" s="2"/>
-      <c r="AA3" s="4"/>
+      <c r="D3" s="11">
+        <v>1</v>
+      </c>
+      <c r="E3" s="1"/>
+      <c r="F3" s="11">
+        <v>1</v>
+      </c>
+      <c r="G3" s="11">
+        <v>1</v>
+      </c>
+      <c r="H3" s="1"/>
+      <c r="I3" s="12">
+        <v>1</v>
+      </c>
+      <c r="J3" s="1"/>
+      <c r="K3" s="1"/>
+      <c r="L3" s="1"/>
+      <c r="M3" s="1"/>
+      <c r="N3" s="1"/>
+      <c r="O3" s="2"/>
+      <c r="P3" s="1"/>
+      <c r="Q3" s="1"/>
+      <c r="R3" s="1"/>
+      <c r="S3" s="1"/>
+      <c r="T3" s="1"/>
+      <c r="U3" s="2"/>
+      <c r="V3" s="1"/>
+      <c r="W3" s="1"/>
+      <c r="X3" s="1"/>
+      <c r="Y3" s="1"/>
+      <c r="Z3" s="1"/>
+      <c r="AA3" s="2"/>
     </row>
     <row r="4" spans="1:27" x14ac:dyDescent="0.25">
-      <c r="A4" s="2">
+      <c r="A4" s="1">
         <v>1</v>
       </c>
       <c r="B4" t="s">
@@ -746,41 +769,41 @@
       <c r="C4">
         <v>1</v>
       </c>
-      <c r="D4" s="2"/>
-      <c r="E4" s="2"/>
-      <c r="F4" s="2"/>
-      <c r="G4" s="2"/>
-      <c r="H4" s="2"/>
-      <c r="I4" s="4"/>
-      <c r="J4" s="2"/>
-      <c r="K4" s="2">
-        <v>1</v>
-      </c>
-      <c r="L4" s="2">
-        <v>1</v>
-      </c>
-      <c r="M4" s="2"/>
-      <c r="N4" s="2">
-        <v>1</v>
-      </c>
-      <c r="O4" s="4">
-        <v>1</v>
-      </c>
-      <c r="P4" s="2"/>
-      <c r="Q4" s="2"/>
-      <c r="R4" s="2"/>
-      <c r="S4" s="2"/>
-      <c r="T4" s="2"/>
-      <c r="U4" s="4"/>
-      <c r="V4" s="2"/>
-      <c r="W4" s="2"/>
-      <c r="X4" s="2"/>
-      <c r="Y4" s="2"/>
-      <c r="Z4" s="2"/>
-      <c r="AA4" s="4"/>
+      <c r="D4" s="1"/>
+      <c r="E4" s="1"/>
+      <c r="F4" s="1"/>
+      <c r="G4" s="1"/>
+      <c r="H4" s="1"/>
+      <c r="I4" s="2"/>
+      <c r="J4" s="1"/>
+      <c r="K4" s="11">
+        <v>1</v>
+      </c>
+      <c r="L4" s="11">
+        <v>1</v>
+      </c>
+      <c r="M4" s="1"/>
+      <c r="N4" s="11">
+        <v>1</v>
+      </c>
+      <c r="O4" s="12">
+        <v>1</v>
+      </c>
+      <c r="P4" s="1"/>
+      <c r="Q4" s="1"/>
+      <c r="R4" s="1"/>
+      <c r="S4" s="1"/>
+      <c r="T4" s="1"/>
+      <c r="U4" s="2"/>
+      <c r="V4" s="1"/>
+      <c r="W4" s="1"/>
+      <c r="X4" s="1"/>
+      <c r="Y4" s="1"/>
+      <c r="Z4" s="1"/>
+      <c r="AA4" s="2"/>
     </row>
     <row r="5" spans="1:27" x14ac:dyDescent="0.25">
-      <c r="A5" s="2">
+      <c r="A5" s="1">
         <v>2</v>
       </c>
       <c r="B5" t="s">
@@ -789,299 +812,299 @@
       <c r="C5">
         <v>1</v>
       </c>
-      <c r="D5" s="6"/>
-      <c r="E5" s="6"/>
-      <c r="F5" s="6"/>
-      <c r="G5" s="6"/>
-      <c r="H5" s="6"/>
-      <c r="I5" s="7"/>
-      <c r="J5" s="6"/>
-      <c r="K5" s="6"/>
-      <c r="L5" s="6"/>
-      <c r="M5" s="6"/>
-      <c r="N5" s="6"/>
-      <c r="O5" s="7"/>
-      <c r="P5" s="6">
-        <v>1</v>
-      </c>
-      <c r="Q5" s="6">
-        <v>1</v>
-      </c>
-      <c r="R5" s="6"/>
-      <c r="S5" s="6">
-        <v>1</v>
-      </c>
-      <c r="T5" s="6">
-        <v>1</v>
-      </c>
-      <c r="U5" s="7"/>
-      <c r="V5" s="2"/>
-      <c r="W5" s="2"/>
-      <c r="X5" s="2"/>
-      <c r="Y5" s="2"/>
-      <c r="Z5" s="2"/>
-      <c r="AA5" s="4"/>
+      <c r="D5" s="3"/>
+      <c r="E5" s="3"/>
+      <c r="F5" s="3"/>
+      <c r="G5" s="3"/>
+      <c r="H5" s="3"/>
+      <c r="I5" s="4"/>
+      <c r="J5" s="3"/>
+      <c r="K5" s="3"/>
+      <c r="L5" s="3"/>
+      <c r="M5" s="3"/>
+      <c r="N5" s="3"/>
+      <c r="O5" s="4"/>
+      <c r="P5" s="10">
+        <v>1</v>
+      </c>
+      <c r="Q5" s="10">
+        <v>1</v>
+      </c>
+      <c r="R5" s="3"/>
+      <c r="S5" s="10">
+        <v>1</v>
+      </c>
+      <c r="T5" s="10">
+        <v>1</v>
+      </c>
+      <c r="U5" s="4"/>
+      <c r="V5" s="1"/>
+      <c r="W5" s="1"/>
+      <c r="X5" s="1"/>
+      <c r="Y5" s="1"/>
+      <c r="Z5" s="1"/>
+      <c r="AA5" s="2"/>
     </row>
     <row r="6" spans="1:27" x14ac:dyDescent="0.25">
-      <c r="A6" s="2">
+      <c r="A6" s="1">
         <v>3</v>
       </c>
-      <c r="B6" t="s">
-        <v>0</v>
+      <c r="B6" s="8" t="s">
+        <v>4</v>
       </c>
       <c r="C6">
         <v>1</v>
       </c>
-      <c r="D6" s="2">
-        <v>1</v>
-      </c>
-      <c r="E6" s="2"/>
-      <c r="F6" s="2"/>
-      <c r="G6" s="2"/>
-      <c r="H6" s="2"/>
-      <c r="I6" s="4"/>
-      <c r="J6" s="8">
-        <v>1</v>
-      </c>
-      <c r="K6" s="2"/>
-      <c r="L6" s="2"/>
-      <c r="M6" s="2"/>
-      <c r="N6" s="2"/>
-      <c r="O6" s="4"/>
-      <c r="P6" s="2">
-        <v>1</v>
-      </c>
-      <c r="Q6" s="2"/>
-      <c r="R6" s="2"/>
-      <c r="S6" s="2"/>
-      <c r="T6" s="2"/>
-      <c r="U6" s="4"/>
-      <c r="V6" s="2">
-        <v>1</v>
-      </c>
-      <c r="W6" s="2"/>
-      <c r="X6" s="2"/>
-      <c r="Y6" s="2"/>
-      <c r="Z6" s="2"/>
-      <c r="AA6" s="4"/>
+      <c r="D6" s="11">
+        <v>1</v>
+      </c>
+      <c r="E6" s="1"/>
+      <c r="F6" s="1"/>
+      <c r="G6" s="1"/>
+      <c r="H6" s="1"/>
+      <c r="I6" s="2"/>
+      <c r="J6" s="5">
+        <v>1</v>
+      </c>
+      <c r="K6" s="1"/>
+      <c r="L6" s="1"/>
+      <c r="M6" s="1"/>
+      <c r="N6" s="1"/>
+      <c r="O6" s="2"/>
+      <c r="P6" s="11">
+        <v>1</v>
+      </c>
+      <c r="Q6" s="1"/>
+      <c r="R6" s="1"/>
+      <c r="S6" s="1"/>
+      <c r="T6" s="1"/>
+      <c r="U6" s="2"/>
+      <c r="V6" s="1">
+        <v>1</v>
+      </c>
+      <c r="W6" s="1"/>
+      <c r="X6" s="1"/>
+      <c r="Y6" s="1"/>
+      <c r="Z6" s="1"/>
+      <c r="AA6" s="2"/>
     </row>
     <row r="7" spans="1:27" x14ac:dyDescent="0.25">
-      <c r="A7" s="2">
+      <c r="A7" s="1">
         <v>4</v>
       </c>
-      <c r="B7" t="s">
-        <v>1</v>
+      <c r="B7" s="8" t="s">
+        <v>5</v>
       </c>
       <c r="C7">
         <v>1</v>
       </c>
-      <c r="D7" s="2"/>
-      <c r="E7" s="8">
-        <v>1</v>
-      </c>
-      <c r="F7" s="2"/>
-      <c r="G7" s="2"/>
-      <c r="H7" s="2"/>
-      <c r="I7" s="4"/>
-      <c r="J7" s="2"/>
-      <c r="K7" s="9">
-        <v>1</v>
-      </c>
-      <c r="L7" s="2"/>
-      <c r="M7" s="2"/>
-      <c r="N7" s="2"/>
-      <c r="O7" s="4"/>
-      <c r="P7" s="2"/>
-      <c r="Q7" s="9">
-        <v>1</v>
-      </c>
-      <c r="R7" s="2"/>
-      <c r="S7" s="2"/>
-      <c r="T7" s="2"/>
-      <c r="U7" s="4"/>
-      <c r="V7" s="2"/>
-      <c r="W7" s="9">
-        <v>1</v>
-      </c>
-      <c r="X7" s="2"/>
-      <c r="Y7" s="2"/>
-      <c r="Z7" s="2"/>
-      <c r="AA7" s="4"/>
+      <c r="D7" s="1"/>
+      <c r="E7" s="5">
+        <v>1</v>
+      </c>
+      <c r="F7" s="1"/>
+      <c r="G7" s="1"/>
+      <c r="H7" s="1"/>
+      <c r="I7" s="2"/>
+      <c r="J7" s="1"/>
+      <c r="K7" s="11">
+        <v>1</v>
+      </c>
+      <c r="L7" s="1"/>
+      <c r="M7" s="1"/>
+      <c r="N7" s="1"/>
+      <c r="O7" s="2"/>
+      <c r="P7" s="1"/>
+      <c r="Q7" s="11">
+        <v>1</v>
+      </c>
+      <c r="R7" s="1"/>
+      <c r="S7" s="1"/>
+      <c r="T7" s="1"/>
+      <c r="U7" s="2"/>
+      <c r="V7" s="1"/>
+      <c r="W7" s="6">
+        <v>1</v>
+      </c>
+      <c r="X7" s="1"/>
+      <c r="Y7" s="1"/>
+      <c r="Z7" s="1"/>
+      <c r="AA7" s="2"/>
     </row>
     <row r="8" spans="1:27" x14ac:dyDescent="0.25">
-      <c r="A8" s="2">
+      <c r="A8" s="1">
         <v>5</v>
       </c>
-      <c r="B8" t="s">
-        <v>2</v>
+      <c r="B8" s="8" t="s">
+        <v>6</v>
       </c>
       <c r="C8">
         <v>1</v>
       </c>
-      <c r="D8" s="2"/>
-      <c r="E8" s="2"/>
-      <c r="F8" s="2">
-        <v>1</v>
-      </c>
-      <c r="G8" s="2"/>
-      <c r="H8" s="2"/>
-      <c r="I8" s="4"/>
-      <c r="J8" s="2"/>
-      <c r="K8" s="2"/>
-      <c r="L8" s="2">
-        <v>1</v>
-      </c>
-      <c r="M8" s="2"/>
-      <c r="N8" s="2"/>
-      <c r="O8" s="4"/>
-      <c r="P8" s="2"/>
-      <c r="Q8" s="2"/>
-      <c r="R8" s="8">
-        <v>1</v>
-      </c>
-      <c r="S8" s="2"/>
-      <c r="T8" s="2"/>
-      <c r="U8" s="4"/>
-      <c r="V8" s="2"/>
-      <c r="W8" s="2"/>
-      <c r="X8" s="2">
-        <v>1</v>
-      </c>
-      <c r="Y8" s="2"/>
-      <c r="Z8" s="2"/>
-      <c r="AA8" s="4"/>
+      <c r="D8" s="1"/>
+      <c r="E8" s="1"/>
+      <c r="F8" s="11">
+        <v>1</v>
+      </c>
+      <c r="G8" s="1"/>
+      <c r="H8" s="1"/>
+      <c r="I8" s="2"/>
+      <c r="J8" s="1"/>
+      <c r="K8" s="1"/>
+      <c r="L8" s="11">
+        <v>1</v>
+      </c>
+      <c r="M8" s="1"/>
+      <c r="N8" s="1"/>
+      <c r="O8" s="2"/>
+      <c r="P8" s="1"/>
+      <c r="Q8" s="1"/>
+      <c r="R8" s="5">
+        <v>1</v>
+      </c>
+      <c r="S8" s="1"/>
+      <c r="T8" s="1"/>
+      <c r="U8" s="2"/>
+      <c r="V8" s="1"/>
+      <c r="W8" s="1"/>
+      <c r="X8" s="1">
+        <v>1</v>
+      </c>
+      <c r="Y8" s="1"/>
+      <c r="Z8" s="1"/>
+      <c r="AA8" s="2"/>
     </row>
     <row r="9" spans="1:27" x14ac:dyDescent="0.25">
-      <c r="A9" s="2">
+      <c r="A9" s="1">
         <v>6</v>
       </c>
-      <c r="B9" t="s">
-        <v>0</v>
+      <c r="B9" s="8" t="s">
+        <v>7</v>
       </c>
       <c r="C9">
         <v>1</v>
       </c>
-      <c r="D9" s="2"/>
-      <c r="E9" s="2"/>
-      <c r="F9" s="2"/>
-      <c r="G9" s="2">
-        <v>1</v>
-      </c>
-      <c r="H9" s="2"/>
-      <c r="I9" s="4"/>
-      <c r="J9" s="2"/>
-      <c r="K9" s="2"/>
-      <c r="L9" s="2"/>
-      <c r="M9" s="8">
-        <v>1</v>
-      </c>
-      <c r="N9" s="2"/>
-      <c r="O9" s="4"/>
-      <c r="P9" s="2"/>
-      <c r="Q9" s="2"/>
-      <c r="R9" s="2"/>
-      <c r="S9" s="2">
-        <v>1</v>
-      </c>
-      <c r="T9" s="2"/>
-      <c r="U9" s="4"/>
-      <c r="V9" s="2"/>
-      <c r="W9" s="2"/>
-      <c r="X9" s="2"/>
-      <c r="Y9" s="2">
-        <v>1</v>
-      </c>
-      <c r="Z9" s="2"/>
-      <c r="AA9" s="4"/>
+      <c r="D9" s="1"/>
+      <c r="E9" s="1"/>
+      <c r="F9" s="1"/>
+      <c r="G9" s="11">
+        <v>1</v>
+      </c>
+      <c r="H9" s="1"/>
+      <c r="I9" s="2"/>
+      <c r="J9" s="1"/>
+      <c r="K9" s="1"/>
+      <c r="L9" s="1"/>
+      <c r="M9" s="5">
+        <v>1</v>
+      </c>
+      <c r="N9" s="1"/>
+      <c r="O9" s="2"/>
+      <c r="P9" s="1"/>
+      <c r="Q9" s="1"/>
+      <c r="R9" s="1"/>
+      <c r="S9" s="11">
+        <v>1</v>
+      </c>
+      <c r="T9" s="1"/>
+      <c r="U9" s="2"/>
+      <c r="V9" s="1"/>
+      <c r="W9" s="1"/>
+      <c r="X9" s="1"/>
+      <c r="Y9" s="1">
+        <v>1</v>
+      </c>
+      <c r="Z9" s="1"/>
+      <c r="AA9" s="2"/>
     </row>
     <row r="10" spans="1:27" x14ac:dyDescent="0.25">
-      <c r="A10" s="2">
+      <c r="A10" s="1">
         <v>7</v>
       </c>
-      <c r="B10" t="s">
-        <v>1</v>
+      <c r="B10" s="8" t="s">
+        <v>8</v>
       </c>
       <c r="C10">
         <v>1</v>
       </c>
-      <c r="D10" s="2"/>
-      <c r="E10" s="2"/>
-      <c r="F10" s="2"/>
-      <c r="G10" s="2"/>
-      <c r="H10" s="8">
-        <v>1</v>
-      </c>
-      <c r="I10" s="4"/>
-      <c r="J10" s="2"/>
-      <c r="K10" s="2"/>
-      <c r="L10" s="2"/>
-      <c r="M10" s="2"/>
-      <c r="N10" s="2">
-        <v>1</v>
-      </c>
-      <c r="O10" s="4"/>
-      <c r="P10" s="2"/>
-      <c r="Q10" s="2"/>
-      <c r="R10" s="2"/>
-      <c r="S10" s="2"/>
-      <c r="T10" s="2">
-        <v>1</v>
-      </c>
-      <c r="U10" s="4"/>
-      <c r="V10" s="2"/>
-      <c r="W10" s="2"/>
-      <c r="X10" s="2"/>
-      <c r="Y10" s="2"/>
-      <c r="Z10" s="2">
-        <v>1</v>
-      </c>
-      <c r="AA10" s="4"/>
+      <c r="D10" s="1"/>
+      <c r="E10" s="1"/>
+      <c r="F10" s="1"/>
+      <c r="G10" s="1"/>
+      <c r="H10" s="5">
+        <v>1</v>
+      </c>
+      <c r="I10" s="2"/>
+      <c r="J10" s="1"/>
+      <c r="K10" s="1"/>
+      <c r="L10" s="1"/>
+      <c r="M10" s="1"/>
+      <c r="N10" s="11">
+        <v>1</v>
+      </c>
+      <c r="O10" s="2"/>
+      <c r="P10" s="1"/>
+      <c r="Q10" s="1"/>
+      <c r="R10" s="1"/>
+      <c r="S10" s="1"/>
+      <c r="T10" s="11">
+        <v>1</v>
+      </c>
+      <c r="U10" s="2"/>
+      <c r="V10" s="1"/>
+      <c r="W10" s="1"/>
+      <c r="X10" s="1"/>
+      <c r="Y10" s="1"/>
+      <c r="Z10" s="1">
+        <v>1</v>
+      </c>
+      <c r="AA10" s="2"/>
     </row>
     <row r="11" spans="1:27" x14ac:dyDescent="0.25">
-      <c r="A11" s="2">
+      <c r="A11" s="1">
         <v>8</v>
       </c>
-      <c r="B11" t="s">
-        <v>2</v>
+      <c r="B11" s="9" t="s">
+        <v>9</v>
       </c>
       <c r="C11">
         <v>1</v>
       </c>
-      <c r="D11" s="2"/>
-      <c r="E11" s="2"/>
-      <c r="F11" s="2"/>
-      <c r="G11" s="2"/>
-      <c r="H11" s="2"/>
-      <c r="I11" s="4">
-        <v>1</v>
-      </c>
-      <c r="J11" s="2"/>
-      <c r="K11" s="2"/>
-      <c r="L11" s="2"/>
-      <c r="M11" s="2"/>
-      <c r="N11" s="2"/>
-      <c r="O11" s="4">
-        <v>1</v>
-      </c>
-      <c r="P11" s="2"/>
-      <c r="Q11" s="2"/>
-      <c r="R11" s="2"/>
-      <c r="S11" s="2"/>
-      <c r="T11" s="2"/>
-      <c r="U11" s="10">
-        <v>1</v>
-      </c>
-      <c r="V11" s="2"/>
-      <c r="W11" s="2"/>
-      <c r="X11" s="2"/>
-      <c r="Y11" s="2"/>
-      <c r="Z11" s="2"/>
-      <c r="AA11" s="4">
+      <c r="D11" s="1"/>
+      <c r="E11" s="1"/>
+      <c r="F11" s="1"/>
+      <c r="G11" s="1"/>
+      <c r="H11" s="1"/>
+      <c r="I11" s="12">
+        <v>1</v>
+      </c>
+      <c r="J11" s="1"/>
+      <c r="K11" s="1"/>
+      <c r="L11" s="1"/>
+      <c r="M11" s="1"/>
+      <c r="N11" s="1"/>
+      <c r="O11" s="12">
+        <v>1</v>
+      </c>
+      <c r="P11" s="1"/>
+      <c r="Q11" s="1"/>
+      <c r="R11" s="1"/>
+      <c r="S11" s="1"/>
+      <c r="T11" s="1"/>
+      <c r="U11" s="7">
+        <v>1</v>
+      </c>
+      <c r="V11" s="1"/>
+      <c r="W11" s="1"/>
+      <c r="X11" s="1"/>
+      <c r="Y11" s="1"/>
+      <c r="Z11" s="1"/>
+      <c r="AA11" s="2">
         <v>1</v>
       </c>
     </row>
     <row r="12" spans="1:27" x14ac:dyDescent="0.25">
-      <c r="A12" s="2">
+      <c r="A12" s="1">
         <v>9</v>
       </c>
       <c r="B12" t="s">
@@ -1090,102 +1113,126 @@
       <c r="C12">
         <v>0</v>
       </c>
-      <c r="D12" s="2"/>
-      <c r="E12" s="2"/>
-      <c r="F12" s="2"/>
-      <c r="G12" s="2"/>
-      <c r="H12" s="2"/>
-      <c r="I12" s="4"/>
-      <c r="J12" s="2"/>
-      <c r="K12" s="2"/>
-      <c r="L12" s="2"/>
-      <c r="M12" s="2"/>
-      <c r="N12" s="2"/>
-      <c r="O12" s="4"/>
-      <c r="P12" s="2"/>
-      <c r="Q12" s="2"/>
-      <c r="R12" s="2"/>
-      <c r="S12" s="2"/>
-      <c r="T12" s="2"/>
-      <c r="U12" s="4"/>
-      <c r="V12" s="2"/>
-      <c r="W12" s="2"/>
-      <c r="X12" s="2"/>
-      <c r="Y12" s="2"/>
-      <c r="Z12" s="2"/>
-      <c r="AA12" s="4"/>
+      <c r="D12" s="1">
+        <v>2</v>
+      </c>
+      <c r="E12" s="1"/>
+      <c r="F12" s="1">
+        <v>13</v>
+      </c>
+      <c r="G12" s="1">
+        <v>10</v>
+      </c>
+      <c r="H12" s="1"/>
+      <c r="I12" s="2">
+        <v>20</v>
+      </c>
+      <c r="J12" s="1"/>
+      <c r="K12" s="1">
+        <v>5</v>
+      </c>
+      <c r="L12" s="1">
+        <v>13</v>
+      </c>
+      <c r="M12" s="1"/>
+      <c r="N12" s="1">
+        <v>12</v>
+      </c>
+      <c r="O12" s="2">
+        <v>20</v>
+      </c>
+      <c r="P12" s="1">
+        <v>2</v>
+      </c>
+      <c r="Q12" s="1">
+        <v>5</v>
+      </c>
+      <c r="R12" s="1"/>
+      <c r="S12" s="1">
+        <v>10</v>
+      </c>
+      <c r="T12" s="1">
+        <v>12</v>
+      </c>
+      <c r="U12" s="2"/>
+      <c r="V12" s="1"/>
+      <c r="W12" s="1"/>
+      <c r="X12" s="1"/>
+      <c r="Y12" s="1"/>
+      <c r="Z12" s="1"/>
+      <c r="AA12" s="2"/>
     </row>
     <row r="13" spans="1:27" x14ac:dyDescent="0.25">
-      <c r="D13" s="2" t="s">
+      <c r="D13" s="1" t="s">
         <v>10</v>
       </c>
-      <c r="E13" s="2" t="s">
+      <c r="E13" s="1" t="s">
         <v>11</v>
       </c>
-      <c r="F13" s="2" t="s">
+      <c r="F13" s="1" t="s">
         <v>12</v>
       </c>
-      <c r="G13" s="2" t="s">
+      <c r="G13" s="1" t="s">
         <v>13</v>
       </c>
-      <c r="H13" s="2" t="s">
+      <c r="H13" s="1" t="s">
         <v>14</v>
       </c>
-      <c r="I13" s="2" t="s">
+      <c r="I13" s="1" t="s">
         <v>15</v>
       </c>
-      <c r="J13" s="2" t="s">
+      <c r="J13" s="1" t="s">
         <v>16</v>
       </c>
-      <c r="K13" s="2" t="s">
+      <c r="K13" s="1" t="s">
         <v>17</v>
       </c>
-      <c r="L13" s="2" t="s">
+      <c r="L13" s="1" t="s">
         <v>18</v>
       </c>
-      <c r="M13" s="2" t="s">
+      <c r="M13" s="1" t="s">
         <v>19</v>
       </c>
-      <c r="N13" s="2" t="s">
+      <c r="N13" s="1" t="s">
         <v>20</v>
       </c>
-      <c r="O13" s="2" t="s">
+      <c r="O13" s="1" t="s">
         <v>22</v>
       </c>
-      <c r="P13" s="2" t="s">
+      <c r="P13" s="1" t="s">
         <v>21</v>
       </c>
-      <c r="Q13" s="2" t="s">
+      <c r="Q13" s="1" t="s">
         <v>23</v>
       </c>
-      <c r="R13" s="2" t="s">
+      <c r="R13" s="1" t="s">
         <v>24</v>
       </c>
-      <c r="S13" s="2" t="s">
+      <c r="S13" s="1" t="s">
         <v>25</v>
       </c>
-      <c r="T13" s="2" t="s">
+      <c r="T13" s="1" t="s">
         <v>26</v>
       </c>
-      <c r="U13" s="2" t="s">
+      <c r="U13" s="1" t="s">
         <v>27</v>
       </c>
-      <c r="V13" s="2" t="s">
+      <c r="V13" s="1" t="s">
         <v>28</v>
       </c>
-      <c r="W13" s="2" t="s">
+      <c r="W13" s="1" t="s">
         <v>29</v>
       </c>
-      <c r="X13" s="2" t="s">
+      <c r="X13" s="1" t="s">
         <v>30</v>
       </c>
-      <c r="Y13" s="2" t="s">
+      <c r="Y13" s="1" t="s">
         <v>31</v>
       </c>
-      <c r="Z13" s="2" t="s">
+      <c r="Z13" s="1" t="s">
         <v>32</v>
       </c>
-      <c r="AA13" s="2" t="s">
+      <c r="AA13" s="1" t="s">
         <v>33</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Sequence of execution of group by and resorting plan construction
</commit_message>
<xml_diff>
--- a/docs/second_step_simplex_table.xlsx
+++ b/docs/second_step_simplex_table.xlsx
@@ -556,8 +556,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:AA13"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="T12" sqref="T12"/>
+    <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="G5" sqref="G5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>